<commit_message>
Consertando coluna Banco Animais
</commit_message>
<xml_diff>
--- a/Bancos/Planilhas/Animais.xlsx
+++ b/Bancos/Planilhas/Animais.xlsx
@@ -1,48 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="planilha" sheetId="1" r:id="rId1"/>
+    <sheet name="planilha" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,30 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -152,7 +211,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -187,7 +245,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -211,6 +268,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -221,31 +279,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -267,7 +325,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -325,7 +383,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -338,12 +396,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -361,50 +420,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="4" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Idade</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Espécie</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Raça</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Cor</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Tamanho</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Tutor</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Horário Chegada</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Horário Saída</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Endereço Histórico</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Conta</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>456</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Rex</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Especie.CACHORRO</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Fila</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Marrom</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Grande</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>123</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Históricos/456.txt</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cadastro funcionando e implementação do tratamento de erro
</commit_message>
<xml_diff>
--- a/Bancos/Planilhas/Animais.xlsx
+++ b/Bancos/Planilhas/Animais.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,6 +549,330 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>520</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Leticia</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Cachorro</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Chihuahua</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Mini</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>510</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Históricos/520.txt</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Laila Said</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Cachorro</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Shar Pei</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Caramelo</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Históricos/2.txt</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Lino</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Azul Russo</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Caramelo</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Grande</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Históricos/3.txt</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Coconut</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Cachorro</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Collie de Pelo Curto</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Caramelo</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Mini</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>10</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Históricos/10.txt</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Galvão</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>13</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Egípcio Mau</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Caramelo</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Grande</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>11</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Históricos/11.txt</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Biscoito</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Exótico de Pelo Curto</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Caramelo</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>12</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Históricos/12.txt</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
atualização da página de agendar e correção de tratamento de erro
</commit_message>
<xml_diff>
--- a/Bancos/Planilhas/Animais.xlsx
+++ b/Bancos/Planilhas/Animais.xlsx
@@ -497,52 +497,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>456</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rex</t>
+          <t>Coconut</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Especie.CACHORRO</t>
+          <t>Cachorro</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Fila</t>
+          <t>Collie de Pelo Curto</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Marrom</t>
+          <t>Caramelo</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Grande</t>
+          <t>Mini</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>123</v>
+        <v>10</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2024-06-11</t>
+          <t>2024-06-12</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2024-06-11</t>
+          <t>2024-06-12</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Históricos/456.txt</t>
+          <t>Históricos/10.txt</t>
         </is>
       </c>
       <c r="L2" t="n">
@@ -551,52 +551,52 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>520</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Leticia</t>
+          <t>Galvão</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cachorro</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Chihuahua</t>
+          <t>Egípcio Mau</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Caramelo</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Mini</t>
+          <t>Grande</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>510</v>
+        <v>11</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2024-06-11</t>
+          <t>2024-06-12</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2024-06-11</t>
+          <t>2024-06-12</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Históricos/520.txt</t>
+          <t>Históricos/11.txt</t>
         </is>
       </c>
       <c r="L3" t="n">
@@ -605,24 +605,24 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Laila Said</t>
+          <t>Biscoito</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Cachorro</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Shar Pei</t>
+          <t>Exótico de Pelo Curto</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -636,21 +636,21 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2024-06-11</t>
+          <t>2024-06-12</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2024-06-11</t>
+          <t>2024-06-12</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Históricos/2.txt</t>
+          <t>Históricos/12.txt</t>
         </is>
       </c>
       <c r="L4" t="n">
@@ -659,24 +659,24 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lino</t>
+          <t>Fofão</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cachorro</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Azul Russo</t>
+          <t>American Bully</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -690,21 +690,21 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-06-16</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-06-16</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Históricos/3.txt</t>
+          <t>Históricos/13.txt</t>
         </is>
       </c>
       <c r="L5" t="n">
@@ -713,24 +713,24 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Coconut</t>
+          <t>Ralf</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cachorro</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Collie de Pelo Curto</t>
+          <t>Chantilly Tiffany</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -740,25 +740,25 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Mini</t>
+          <t>Pequeno</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-06-16</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-06-16</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Históricos/10.txt</t>
+          <t>Históricos/14.txt</t>
         </is>
       </c>
       <c r="L6" t="n">
@@ -767,24 +767,24 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Galvão</t>
+          <t>Jujuba</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cachorro</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Egípcio Mau</t>
+          <t>Bloodhound ou Cão-de-Santo-Humberto</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -794,25 +794,25 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Grande</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-06-16</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-06-16</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Históricos/11.txt</t>
+          <t>Históricos/15.txt</t>
         </is>
       </c>
       <c r="L7" t="n">
@@ -821,24 +821,24 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Biscoito</t>
+          <t>Luna</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cachorro</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Exótico de Pelo Curto</t>
+          <t>Boykin spaniel</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -848,25 +848,25 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Pequeno</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-06-16</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-06-16</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Históricos/12.txt</t>
+          <t>Históricos/16.txt</t>
         </is>
       </c>
       <c r="L8" t="n">

</xml_diff>

<commit_message>
ultimas modificações das páginas
</commit_message>
<xml_diff>
--- a/Bancos/Planilhas/Animais.xlsx
+++ b/Bancos/Planilhas/Animais.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,8 +529,10 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>15</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -585,8 +587,10 @@
           <t>Pequeno</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>16</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -610,16 +614,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Leticia</t>
+          <t>Mel</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -628,262 +632,40 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Chihuahua</t>
+          <t>Cão-pelado-peruano</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Caramelo</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Mini</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>510</v>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1647894877</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2024-06-19</t>
+          <t>2024-06-20</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2024-06-19</t>
+          <t>2024-06-20</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Históricos/520.txt</t>
+          <t>Históricos/34.txt</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Jade</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Cachorro</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Boiadeiro de Appenzeller</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Caramelo</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Pequeno</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>22</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Históricos/22.txt</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>520</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Leticia</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>90</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Cachorro</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Chihuahua</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Mini</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>510</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Históricos/520.txt</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>520</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Leticia</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>90</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Cachorro</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Chihuahua</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Mini</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>510</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Históricos/520.txt</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>520</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Leticia</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>90</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Cachorro</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Chihuahua</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Mini</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>510</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Históricos/520.txt</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>